<commit_message>
Cganges to products and organisations
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Organisation_Defs.xlsx
+++ b/inputs/AddictO_Organisation_Defs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\User3\Work\Github\addiction-ontology\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AD496F-DAA6-4EE1-AD77-7ED08CDBF0F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="4" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="167">
   <si>
     <t>ID</t>
   </si>
@@ -490,13 +491,52 @@
   </si>
   <si>
     <t>A material entity which can play roles, has members, and has a set of organization rules. Members of organizations are either organizations themselves or individual people. Members can bear specific organization member roles that are determined in the organization rules. The organization rules also determine how decisions are made on behalf of the organization by the organization members.</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>An aggregate of organisations that manufacture, prepare for sale, distribute, market or promote products or services.</t>
+  </si>
+  <si>
+    <t>E-cigarette industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have added here promotion of - this sets industry apart from manufactureres of but also includes these types of company. </t>
+  </si>
+  <si>
+    <t>E-Cig industry</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>An industry in which the product is electronic cigarettes or e-liquid.</t>
+  </si>
+  <si>
+    <t>Independent e-cigarette industry</t>
+  </si>
+  <si>
+    <t>Independent e-cigarette company</t>
+  </si>
+  <si>
+    <t>(Note: This is intended to include ownership, investment or sharing of resources.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An e-cigarette company that has no commercial or financial association with a tobacco company. </t>
+  </si>
+  <si>
+    <t>An e-cigarette industry that has only independent e-cigarette companies as a part.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,13 +569,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -544,30 +577,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -582,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -603,7 +629,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -612,23 +641,32 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -964,764 +1002,877 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="A26:XFD1346"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16" style="11" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="64.42578125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="16" style="11" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="48.28515625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="44.140625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="11"/>
-    <col min="13" max="13" width="18.42578125" style="11" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="11"/>
-    <col min="16" max="16" width="13.42578125" style="11" customWidth="1"/>
-    <col min="17" max="17" width="37.140625" style="11" customWidth="1"/>
-    <col min="18" max="18" width="48.7109375" style="11" customWidth="1"/>
-    <col min="19" max="19" width="24.7109375" style="11" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="16" style="20" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="64.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="16" style="20" customWidth="1"/>
+    <col min="7" max="7" width="35.453125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="48.26953125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="29.7265625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="44.1796875" style="20" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="20"/>
+    <col min="13" max="13" width="18.453125" style="20" customWidth="1"/>
+    <col min="14" max="15" width="9.1796875" style="20"/>
+    <col min="16" max="16" width="13.453125" style="20" customWidth="1"/>
+    <col min="17" max="17" width="37.1796875" style="20" customWidth="1"/>
+    <col min="18" max="18" width="48.7265625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="24.7265625" style="20" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:19" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="12"/>
-    </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="10"/>
+    </row>
+    <row r="3" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12">
-        <v>1</v>
-      </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10">
+        <v>1</v>
+      </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12">
-        <v>1</v>
-      </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12">
-        <v>1</v>
-      </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12" t="s">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10">
+        <v>1</v>
+      </c>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12">
-        <v>1</v>
-      </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+    <row r="7" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12">
-        <v>1</v>
-      </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12" t="s">
+      <c r="J7" s="16"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10">
+        <v>1</v>
+      </c>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12">
-        <v>1</v>
-      </c>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10">
+        <v>1</v>
+      </c>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="10" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15" t="s">
+    <row r="9" spans="1:19" s="9" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15">
-        <v>1</v>
-      </c>
-      <c r="O9" s="15"/>
-      <c r="P9" s="14" t="s">
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17">
+        <v>1</v>
+      </c>
+      <c r="O9" s="17"/>
+      <c r="P9" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-    </row>
-    <row r="10" spans="1:19" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="10" t="s">
+      <c r="Q9" s="12"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+    </row>
+    <row r="10" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+    </row>
+    <row r="11" spans="1:19" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14">
+        <v>1</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q11" s="14"/>
+      <c r="S11" s="14"/>
+    </row>
+    <row r="12" spans="1:19" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="S12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14">
+        <v>1</v>
+      </c>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="R13" s="19"/>
+    </row>
+    <row r="14" spans="1:19" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="12"/>
-    </row>
-    <row r="11" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="Q14" s="10"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="10"/>
+    </row>
+    <row r="15" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P15" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="S11" s="12"/>
-    </row>
-    <row r="12" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10" t="s">
+      <c r="S15" s="10"/>
+    </row>
+    <row r="16" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="P16" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="R12" s="13"/>
-      <c r="S12" s="12"/>
-    </row>
-    <row r="13" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="R16" s="16"/>
+      <c r="S16" s="10"/>
+    </row>
+    <row r="17" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P13" s="10" t="s">
+      <c r="P17" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="S13" s="12"/>
-    </row>
-    <row r="14" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="S17" s="10"/>
+    </row>
+    <row r="18" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="P18" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="S14" s="12"/>
-    </row>
-    <row r="15" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="S18" s="10"/>
+    </row>
+    <row r="19" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P15" s="10" t="s">
+      <c r="P19" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q15" s="12"/>
-      <c r="S15" s="12"/>
-    </row>
-    <row r="16" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="Q19" s="10"/>
+      <c r="S19" s="10"/>
+    </row>
+    <row r="20" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="P20" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="S16" s="12"/>
-    </row>
-    <row r="17" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="S20" s="10"/>
+    </row>
+    <row r="21" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="P21" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="S17" s="12"/>
-    </row>
-    <row r="18" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="10" t="s">
+      <c r="S21" s="10"/>
+    </row>
+    <row r="22" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P18" s="10" t="s">
+      <c r="P22" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="R18" s="13"/>
-      <c r="S18" s="12"/>
-    </row>
-    <row r="19" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="R22" s="16"/>
+      <c r="S22" s="10"/>
+    </row>
+    <row r="23" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="P23" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q19" s="12"/>
-      <c r="S19" s="12"/>
-    </row>
-    <row r="20" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="10" t="s">
+      <c r="Q23" s="10"/>
+      <c r="S23" s="10"/>
+    </row>
+    <row r="24" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P20" s="10" t="s">
+      <c r="P24" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="R20" s="13"/>
-    </row>
-    <row r="21" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="R24" s="16"/>
+    </row>
+    <row r="25" spans="1:19" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I25" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="P21" s="10" t="s">
+      <c r="P25" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="10" t="s">
+    <row r="26" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P22" s="10" t="s">
+      <c r="P26" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="13"/>
-    </row>
-    <row r="23" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="10" t="s">
+      <c r="Q26" s="10"/>
+      <c r="R26" s="16"/>
+    </row>
+    <row r="27" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
+      <c r="B27" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P23" s="10" t="s">
+      <c r="P27" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="13"/>
-    </row>
-    <row r="24" spans="1:19" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="Q27" s="10"/>
+      <c r="R27" s="16"/>
+    </row>
+    <row r="28" spans="1:19" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="12"/>
-    </row>
-    <row r="25" spans="1:19" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="10" t="s">
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P25" s="10" t="s">
+      <c r="P29" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q25" s="12"/>
-      <c r="R25" s="13"/>
-    </row>
-    <row r="26" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="P26" s="10" t="s">
+      <c r="Q29" s="10"/>
+      <c r="R29" s="16"/>
+    </row>
+    <row r="30" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="16"/>
+      <c r="P30" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="13"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11">
-        <v>1</v>
-      </c>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-    </row>
-    <row r="28" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="P28" s="10" t="s">
+    <row r="31" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="16"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20">
+        <v>1</v>
+      </c>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+      <c r="O31" s="20"/>
+      <c r="P31" s="20"/>
+    </row>
+    <row r="32" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="16"/>
+      <c r="P32" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
-      <c r="P29" s="10" t="s">
+    <row r="33" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="16"/>
+      <c r="P33" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="P30" s="10" t="s">
+    <row r="34" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="16"/>
+      <c r="P34" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="13"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-    </row>
-    <row r="32" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-      <c r="P32" s="10" t="s">
+    <row r="35" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="16"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+    </row>
+    <row r="36" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="16"/>
+      <c r="P36" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-    </row>
-    <row r="34" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="13"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-    </row>
-    <row r="35" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="13"/>
-      <c r="Q35" s="11"/>
-    </row>
-    <row r="36" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="13"/>
-    </row>
-    <row r="37" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="13"/>
-    </row>
-    <row r="38" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="13"/>
-    </row>
-    <row r="39" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="13"/>
-    </row>
-    <row r="40" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="13"/>
-    </row>
-    <row r="41" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
-    </row>
-    <row r="42" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
-    </row>
-    <row r="43" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="13"/>
-    </row>
-    <row r="44" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="R44" s="11"/>
-    </row>
-    <row r="45" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="13"/>
-      <c r="Q45" s="11"/>
-    </row>
-    <row r="46" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="13"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-    </row>
-    <row r="47" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="13"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-    </row>
-    <row r="48" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-    </row>
-    <row r="49" spans="2:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="13"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-    </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B50" s="13"/>
+    <row r="37" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="16"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+    </row>
+    <row r="38" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="16"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+    </row>
+    <row r="39" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="16"/>
+      <c r="Q39" s="20"/>
+    </row>
+    <row r="40" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="16"/>
+    </row>
+    <row r="41" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="16"/>
+    </row>
+    <row r="42" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="16"/>
+    </row>
+    <row r="44" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="16"/>
+    </row>
+    <row r="45" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="16"/>
+    </row>
+    <row r="47" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="16"/>
+    </row>
+    <row r="48" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="R48" s="20"/>
+    </row>
+    <row r="49" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="16"/>
+      <c r="Q49" s="20"/>
+    </row>
+    <row r="50" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="16"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="20"/>
+    </row>
+    <row r="51" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="16"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+    </row>
+    <row r="52" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="20"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="20"/>
+      <c r="R52" s="20"/>
+    </row>
+    <row r="53" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="16"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="20"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B54" s="16"/>
     </row>
   </sheetData>
-  <sortState ref="A2:S2822">
-    <sortCondition ref="F2:F2822"/>
-    <sortCondition descending="1" ref="N2:N2822"/>
-    <sortCondition ref="B2:B2822"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S2826">
+    <sortCondition ref="F2:F2826"/>
+    <sortCondition descending="1" ref="N2:N2826"/>
+    <sortCondition ref="B2:B2826"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1729,23 +1880,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.453125" style="4" customWidth="1"/>
     <col min="3" max="3" width="93" style="4" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="45.1796875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
@@ -1759,7 +1910,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1770,7 +1921,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1781,7 +1932,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1795,7 +1946,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -1806,7 +1957,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>56</v>
       </c>
@@ -1820,7 +1971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>70</v>
       </c>
@@ -1831,7 +1982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -1842,7 +1993,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>63</v>
       </c>
@@ -1853,7 +2004,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
@@ -1864,7 +2015,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>65</v>
       </c>
@@ -1875,7 +2026,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>62</v>
       </c>
@@ -1886,7 +2037,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -1897,7 +2048,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>67</v>
       </c>
@@ -1908,7 +2059,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>97</v>
       </c>
@@ -1919,7 +2070,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>98</v>
       </c>
@@ -1930,7 +2081,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>99</v>
       </c>
@@ -1941,7 +2092,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>100</v>
       </c>
@@ -1952,7 +2103,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>144</v>
       </c>
@@ -1970,29 +2121,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="36.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.26953125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="36.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.26953125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.26953125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2030,7 +2181,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2044,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2058,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2075,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2086,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -2100,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2117,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2131,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -2148,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="40.5" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -2168,14 +2319,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2183,19 +2334,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="43.28515625" customWidth="1"/>
+    <col min="11" max="11" width="43.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
@@ -2230,7 +2381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2241,7 +2392,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2258,7 +2409,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2275,7 +2426,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2292,7 +2443,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2309,7 +2460,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2326,7 +2477,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2343,7 +2494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2360,7 +2511,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2377,7 +2528,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2394,7 +2545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2420,7 +2571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2446,7 +2597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2472,7 +2623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2498,7 +2649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2524,7 +2675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2550,7 +2701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2576,7 +2727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2602,7 +2753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2628,7 +2779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2654,7 +2805,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2680,7 +2831,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2706,7 +2857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2732,7 +2883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2758,7 +2909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2784,7 +2935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2810,7 +2961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2836,7 +2987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2862,7 +3013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Additions Products & Organisations
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Organisation_Defs.xlsx
+++ b/inputs/AddictO_Organisation_Defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharoncox/Documents/GitHub/addiction-ontology/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBDDB3F-0205-44C5-AD9F-AA7AEAB4A793}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CEC57A-7C37-1C4F-87F9-44DB5890D96F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="224">
   <si>
     <t>ID</t>
   </si>
@@ -677,6 +677,30 @@
   </si>
   <si>
     <t>An aggregate of organisations.</t>
+  </si>
+  <si>
+    <t>Cannabis retail outlet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A cannabis retailer that has a physical outlet. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannabis retailer </t>
+  </si>
+  <si>
+    <t>Cannabis retailer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A cannabis company that predominantly sells cannabis products and related merchandise. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannabis company </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A cannabis industry that is engaged in the growth, manufacture, preparation for sale, shipment, advertisement, or distribution of cannabis products. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannabis industry </t>
   </si>
 </sst>
 </file>
@@ -1208,35 +1232,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" style="19" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="77.6328125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="23.81640625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="19" customWidth="1"/>
+    <col min="3" max="3" width="77.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="19" customWidth="1"/>
     <col min="6" max="6" width="16" style="19" customWidth="1"/>
-    <col min="7" max="7" width="35.453125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="48.36328125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="23.453125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="29.6328125" style="19" customWidth="1"/>
-    <col min="11" max="11" width="44.1796875" style="19" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="19"/>
-    <col min="13" max="13" width="18.453125" style="19" customWidth="1"/>
-    <col min="14" max="15" width="9.1796875" style="19"/>
-    <col min="16" max="16" width="13.453125" style="19" customWidth="1"/>
-    <col min="17" max="17" width="37.1796875" style="19" customWidth="1"/>
-    <col min="18" max="18" width="48.6328125" style="19" customWidth="1"/>
-    <col min="19" max="19" width="24.6328125" style="19" customWidth="1"/>
-    <col min="20" max="16384" width="9.1796875" style="19"/>
+    <col min="7" max="7" width="35.5" style="19" customWidth="1"/>
+    <col min="8" max="8" width="48.33203125" style="19" customWidth="1"/>
+    <col min="9" max="9" width="23.5" style="19" customWidth="1"/>
+    <col min="10" max="10" width="29.6640625" style="19" customWidth="1"/>
+    <col min="11" max="11" width="44.1640625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="19"/>
+    <col min="13" max="13" width="18.5" style="19" customWidth="1"/>
+    <col min="14" max="15" width="9.1640625" style="19"/>
+    <col min="16" max="16" width="13.5" style="19" customWidth="1"/>
+    <col min="17" max="17" width="37.1640625" style="19" customWidth="1"/>
+    <col min="18" max="18" width="48.6640625" style="19" customWidth="1"/>
+    <col min="19" max="19" width="24.6640625" style="19" customWidth="1"/>
+    <col min="20" max="16384" width="9.1640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="15" customFormat="1" ht="29">
+    <row r="1" spans="1:19" s="15" customFormat="1" ht="32">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1292,7 +1316,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="9" customFormat="1">
+    <row r="2" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
         <v>103</v>
@@ -1324,7 +1348,7 @@
       <c r="R2" s="16"/>
       <c r="S2" s="10"/>
     </row>
-    <row r="3" spans="1:19" s="9" customFormat="1" ht="29">
+    <row r="3" spans="1:19" s="9" customFormat="1" ht="32">
       <c r="B3" s="10" t="s">
         <v>106</v>
       </c>
@@ -1349,7 +1373,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="9" customFormat="1">
+    <row r="4" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B4" s="10" t="s">
         <v>107</v>
       </c>
@@ -1374,7 +1398,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="9" customFormat="1">
+    <row r="5" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B5" s="10" t="s">
         <v>108</v>
       </c>
@@ -1399,7 +1423,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="9" customFormat="1">
+    <row r="6" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B6" s="10" t="s">
         <v>109</v>
       </c>
@@ -1424,7 +1448,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="9" customFormat="1" ht="29">
+    <row r="7" spans="1:19" s="9" customFormat="1" ht="32">
       <c r="B7" s="10" t="s">
         <v>110</v>
       </c>
@@ -1451,7 +1475,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="9" customFormat="1">
+    <row r="8" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B8" s="10" t="s">
         <v>112</v>
       </c>
@@ -1476,7 +1500,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="9" customFormat="1" ht="72.5">
+    <row r="9" spans="1:19" s="9" customFormat="1" ht="64">
       <c r="A9" s="11"/>
       <c r="B9" s="17" t="s">
         <v>4</v>
@@ -1517,7 +1541,7 @@
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
     </row>
-    <row r="10" spans="1:19" s="9" customFormat="1">
+    <row r="10" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="A10" s="11"/>
       <c r="B10" s="17" t="s">
         <v>213</v>
@@ -1544,7 +1568,7 @@
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
     </row>
-    <row r="11" spans="1:19" s="9" customFormat="1" ht="29">
+    <row r="11" spans="1:19" s="9" customFormat="1" ht="32">
       <c r="A11" s="11"/>
       <c r="B11" s="17" t="s">
         <v>153</v>
@@ -1575,7 +1599,7 @@
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
     </row>
-    <row r="12" spans="1:19" s="21" customFormat="1">
+    <row r="12" spans="1:19" s="21" customFormat="1" ht="16">
       <c r="B12" s="22" t="s">
         <v>172</v>
       </c>
@@ -1608,7 +1632,7 @@
       <c r="Q12" s="22"/>
       <c r="R12" s="23"/>
     </row>
-    <row r="13" spans="1:19" s="13" customFormat="1" ht="43.5">
+    <row r="13" spans="1:19" s="13" customFormat="1" ht="32">
       <c r="B13" s="14" t="s">
         <v>155</v>
       </c>
@@ -1646,7 +1670,7 @@
       <c r="Q13" s="14"/>
       <c r="S13" s="14"/>
     </row>
-    <row r="14" spans="1:19" s="24" customFormat="1" ht="14">
+    <row r="14" spans="1:19" s="24" customFormat="1" ht="16">
       <c r="B14" s="25" t="s">
         <v>161</v>
       </c>
@@ -1674,7 +1698,7 @@
       <c r="Q14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" s="24" customFormat="1" ht="42">
+    <row r="15" spans="1:19" s="24" customFormat="1" ht="48">
       <c r="B15" s="25" t="s">
         <v>162</v>
       </c>
@@ -1710,7 +1734,7 @@
       </c>
       <c r="R15" s="31"/>
     </row>
-    <row r="16" spans="1:19" s="27" customFormat="1" ht="14">
+    <row r="16" spans="1:19" s="27" customFormat="1" ht="16">
       <c r="B16" s="28" t="s">
         <v>166</v>
       </c>
@@ -1745,7 +1769,7 @@
       <c r="R16" s="30"/>
       <c r="S16" s="28"/>
     </row>
-    <row r="17" spans="1:19" s="27" customFormat="1" ht="14">
+    <row r="17" spans="1:19" s="27" customFormat="1" ht="16">
       <c r="B17" s="28" t="s">
         <v>175</v>
       </c>
@@ -1780,7 +1804,7 @@
       <c r="Q17" s="28"/>
       <c r="R17" s="30"/>
     </row>
-    <row r="18" spans="1:19" s="20" customFormat="1" ht="29">
+    <row r="18" spans="1:19" s="20" customFormat="1" ht="32">
       <c r="A18" s="21"/>
       <c r="B18" s="22" t="s">
         <v>168</v>
@@ -1819,7 +1843,7 @@
       <c r="R18" s="23"/>
       <c r="S18" s="21"/>
     </row>
-    <row r="19" spans="1:19" s="20" customFormat="1">
+    <row r="19" spans="1:19" s="20" customFormat="1" ht="16">
       <c r="A19" s="21"/>
       <c r="B19" s="22" t="s">
         <v>170</v>
@@ -1856,7 +1880,7 @@
       <c r="R19" s="23"/>
       <c r="S19" s="21"/>
     </row>
-    <row r="20" spans="1:19" s="27" customFormat="1" ht="84">
+    <row r="20" spans="1:19" s="27" customFormat="1" ht="80">
       <c r="A20" s="28"/>
       <c r="B20" s="29" t="s">
         <v>176</v>
@@ -1894,7 +1918,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="27" customFormat="1" ht="14">
+    <row r="21" spans="1:19" s="27" customFormat="1" ht="16">
       <c r="A21" s="28"/>
       <c r="B21" s="29" t="s">
         <v>187</v>
@@ -1926,7 +1950,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="27" customFormat="1" ht="14">
+    <row r="22" spans="1:19" s="27" customFormat="1" ht="16">
       <c r="A22" s="28"/>
       <c r="B22" s="29" t="s">
         <v>186</v>
@@ -1962,7 +1986,7 @@
       <c r="Q22" s="28"/>
       <c r="R22" s="34"/>
     </row>
-    <row r="23" spans="1:19" s="27" customFormat="1" ht="14">
+    <row r="23" spans="1:19" s="27" customFormat="1" ht="16">
       <c r="A23" s="28"/>
       <c r="B23" s="29" t="s">
         <v>190</v>
@@ -1997,7 +2021,7 @@
       </c>
       <c r="Q23" s="28"/>
     </row>
-    <row r="24" spans="1:19" s="11" customFormat="1" ht="43.5">
+    <row r="24" spans="1:19" s="11" customFormat="1" ht="48">
       <c r="A24" s="12"/>
       <c r="B24" s="35" t="s">
         <v>113</v>
@@ -2024,7 +2048,7 @@
       <c r="R24" s="18"/>
       <c r="S24" s="12"/>
     </row>
-    <row r="25" spans="1:19" s="9" customFormat="1">
+    <row r="25" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B25" s="9" t="s">
         <v>117</v>
       </c>
@@ -2036,7 +2060,7 @@
       </c>
       <c r="S25" s="10"/>
     </row>
-    <row r="26" spans="1:19" s="9" customFormat="1" ht="29">
+    <row r="26" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="A26" s="10"/>
       <c r="B26" s="9" t="s">
         <v>118</v>
@@ -2053,7 +2077,7 @@
       <c r="R26" s="16"/>
       <c r="S26" s="10"/>
     </row>
-    <row r="27" spans="1:19" s="9" customFormat="1">
+    <row r="27" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B27" s="9" t="s">
         <v>120</v>
       </c>
@@ -2065,7 +2089,7 @@
       </c>
       <c r="S27" s="10"/>
     </row>
-    <row r="28" spans="1:19" s="9" customFormat="1">
+    <row r="28" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B28" s="9" t="s">
         <v>121</v>
       </c>
@@ -2077,7 +2101,7 @@
       </c>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="1:19" s="9" customFormat="1">
+    <row r="29" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B29" s="9" t="s">
         <v>122</v>
       </c>
@@ -2090,7 +2114,7 @@
       <c r="Q29" s="10"/>
       <c r="S29" s="10"/>
     </row>
-    <row r="30" spans="1:19" s="9" customFormat="1">
+    <row r="30" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B30" s="9" t="s">
         <v>123</v>
       </c>
@@ -2102,7 +2126,7 @@
       </c>
       <c r="S30" s="10"/>
     </row>
-    <row r="31" spans="1:19" s="9" customFormat="1">
+    <row r="31" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="B31" s="9" t="s">
         <v>124</v>
       </c>
@@ -2114,7 +2138,7 @@
       </c>
       <c r="S31" s="10"/>
     </row>
-    <row r="32" spans="1:19" s="9" customFormat="1">
+    <row r="32" spans="1:19" s="9" customFormat="1" ht="16">
       <c r="A32" s="10"/>
       <c r="B32" s="9" t="s">
         <v>125</v>
@@ -2128,7 +2152,7 @@
       <c r="R32" s="16"/>
       <c r="S32" s="10"/>
     </row>
-    <row r="33" spans="1:20" s="9" customFormat="1">
+    <row r="33" spans="1:20" s="9" customFormat="1" ht="16">
       <c r="B33" s="9" t="s">
         <v>126</v>
       </c>
@@ -2141,7 +2165,7 @@
       <c r="Q33" s="10"/>
       <c r="S33" s="10"/>
     </row>
-    <row r="34" spans="1:20" s="9" customFormat="1" ht="29">
+    <row r="34" spans="1:20" s="9" customFormat="1" ht="16">
       <c r="A34" s="10"/>
       <c r="B34" s="9" t="s">
         <v>127</v>
@@ -2154,7 +2178,7 @@
       </c>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="1:20" s="9" customFormat="1" ht="29">
+    <row r="35" spans="1:20" s="9" customFormat="1" ht="32">
       <c r="B35" s="9" t="s">
         <v>128</v>
       </c>
@@ -2168,7 +2192,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="9" customFormat="1">
+    <row r="36" spans="1:20" s="9" customFormat="1" ht="16">
       <c r="A36" s="10"/>
       <c r="B36" s="9" t="s">
         <v>130</v>
@@ -2182,7 +2206,7 @@
       <c r="Q36" s="10"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" spans="1:20" s="9" customFormat="1">
+    <row r="37" spans="1:20" s="9" customFormat="1" ht="16">
       <c r="A37" s="10"/>
       <c r="B37" s="9" t="s">
         <v>131</v>
@@ -2196,7 +2220,7 @@
       <c r="Q37" s="10"/>
       <c r="R37" s="16"/>
     </row>
-    <row r="38" spans="1:20" s="9" customFormat="1" ht="43.5">
+    <row r="38" spans="1:20" s="9" customFormat="1" ht="48">
       <c r="B38" s="19" t="s">
         <v>57</v>
       </c>
@@ -2218,7 +2242,7 @@
       <c r="P38" s="19"/>
       <c r="Q38" s="10"/>
     </row>
-    <row r="39" spans="1:20" s="9" customFormat="1">
+    <row r="39" spans="1:20" s="9" customFormat="1" ht="16">
       <c r="A39" s="10"/>
       <c r="B39" s="9" t="s">
         <v>132</v>
@@ -2232,7 +2256,7 @@
       <c r="Q39" s="10"/>
       <c r="R39" s="16"/>
     </row>
-    <row r="40" spans="1:20" s="32" customFormat="1">
+    <row r="40" spans="1:20" s="32" customFormat="1" ht="16">
       <c r="B40" s="23" t="s">
         <v>184</v>
       </c>
@@ -2252,7 +2276,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="32" customFormat="1">
+    <row r="41" spans="1:20" s="32" customFormat="1" ht="16">
       <c r="B41" s="23" t="s">
         <v>202</v>
       </c>
@@ -2282,7 +2306,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="32" customFormat="1" ht="29">
+    <row r="42" spans="1:20" s="32" customFormat="1" ht="32">
       <c r="B42" s="23" t="s">
         <v>192</v>
       </c>
@@ -2311,7 +2335,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="32" customFormat="1" ht="29">
+    <row r="43" spans="1:20" s="32" customFormat="1" ht="32">
       <c r="B43" s="23" t="s">
         <v>196</v>
       </c>
@@ -2340,7 +2364,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="21" customFormat="1" ht="29">
+    <row r="44" spans="1:20" s="21" customFormat="1" ht="32">
       <c r="B44" s="22" t="s">
         <v>200</v>
       </c>
@@ -2372,7 +2396,7 @@
       <c r="R44" s="33"/>
       <c r="S44" s="22"/>
     </row>
-    <row r="45" spans="1:20" s="21" customFormat="1" ht="29">
+    <row r="45" spans="1:20" s="21" customFormat="1" ht="32">
       <c r="A45" s="22"/>
       <c r="B45" s="21" t="s">
         <v>203</v>
@@ -2394,7 +2418,7 @@
       </c>
       <c r="Q45" s="22"/>
     </row>
-    <row r="46" spans="1:20" s="21" customFormat="1">
+    <row r="46" spans="1:20" s="21" customFormat="1" ht="16">
       <c r="A46" s="33"/>
       <c r="B46" s="22" t="s">
         <v>205</v>
@@ -2427,7 +2451,7 @@
       </c>
       <c r="S46" s="22"/>
     </row>
-    <row r="47" spans="1:20" s="21" customFormat="1" ht="43.5">
+    <row r="47" spans="1:20" s="21" customFormat="1" ht="32">
       <c r="A47" s="22"/>
       <c r="B47" s="21" t="s">
         <v>210</v>
@@ -2452,29 +2476,66 @@
       </c>
       <c r="T47" s="22"/>
     </row>
-    <row r="48" spans="1:20" s="9" customFormat="1">
-      <c r="B48" s="16"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
-      <c r="N48" s="19"/>
-      <c r="O48" s="19"/>
-      <c r="P48" s="19"/>
-    </row>
-    <row r="49" spans="1:18" s="9" customFormat="1">
-      <c r="B49" s="16"/>
-      <c r="Q49" s="19"/>
-    </row>
-    <row r="50" spans="1:18" s="9" customFormat="1">
-      <c r="B50" s="16"/>
+    <row r="48" spans="1:20" s="21" customFormat="1" ht="16">
+      <c r="B48" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="O48" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="P48" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" s="32" customFormat="1" ht="16">
+      <c r="B49" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="O49" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="P49" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q49" s="33"/>
+    </row>
+    <row r="50" spans="1:18" s="32" customFormat="1" ht="16">
+      <c r="B50" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="O50" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="P50" s="32" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="51" spans="1:18" s="9" customFormat="1">
       <c r="B51" s="16"/>
@@ -2583,7 +2644,7 @@
       <c r="B64" s="16"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S2836">
+  <sortState ref="A2:S2836">
     <sortCondition ref="F2:F2836"/>
     <sortCondition descending="1" ref="N2:N2836"/>
     <sortCondition ref="B2:B2836"/>
@@ -2601,16 +2662,16 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="93" style="4" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="4" width="45.1640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="16">
       <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
@@ -2624,7 +2685,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="43.5">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="48">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2635,7 +2696,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="29">
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2646,7 +2707,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="58">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="64">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2660,7 +2721,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="29">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A5" s="5" t="s">
         <v>55</v>
       </c>
@@ -2671,7 +2732,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="43.5">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A6" s="5" t="s">
         <v>56</v>
       </c>
@@ -2685,7 +2746,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="29">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A7" s="5" t="s">
         <v>70</v>
       </c>
@@ -2696,7 +2757,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="43.5">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -2707,7 +2768,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
         <v>63</v>
       </c>
@@ -2718,7 +2779,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="29">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
@@ -2729,7 +2790,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="29">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A11" s="5" t="s">
         <v>65</v>
       </c>
@@ -2740,7 +2801,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
         <v>62</v>
       </c>
@@ -2751,7 +2812,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="29">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="32">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -2762,7 +2823,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="58">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="48">
       <c r="A14" s="5" t="s">
         <v>67</v>
       </c>
@@ -2773,7 +2834,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="29">
+    <row r="15" spans="1:4" ht="16">
       <c r="A15" s="5" t="s">
         <v>97</v>
       </c>
@@ -2784,7 +2845,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="16">
       <c r="A16" s="5" t="s">
         <v>98</v>
       </c>
@@ -2795,7 +2856,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="16">
       <c r="A17" s="5" t="s">
         <v>99</v>
       </c>
@@ -2806,7 +2867,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" ht="16">
       <c r="A18" s="5" t="s">
         <v>100</v>
       </c>
@@ -2817,7 +2878,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="29">
+    <row r="19" spans="1:3" ht="32">
       <c r="A19" s="5" t="s">
         <v>143</v>
       </c>
@@ -2842,22 +2903,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="36.453125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.36328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.453125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.36328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.36328125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="36.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="16">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2895,7 +2956,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="43.5">
+    <row r="2" spans="1:12" ht="48">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2909,7 +2970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="58">
+    <row r="3" spans="1:12" ht="48">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2923,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="43.5">
+    <row r="4" spans="1:12" ht="48">
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -2940,7 +3001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="58">
+    <row r="5" spans="1:12" ht="48">
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
@@ -2951,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.5">
+    <row r="6" spans="1:12" ht="48">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
@@ -2965,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="43.5">
+    <row r="7" spans="1:12" ht="48">
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
@@ -2982,7 +3043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" ht="16">
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2996,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="43.5">
+    <row r="9" spans="1:12" ht="48">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -3013,7 +3074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="40.5">
+    <row r="10" spans="1:12" ht="42">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3040,7 +3101,7 @@
       <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3055,9 +3116,9 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="11" max="11" width="43.36328125" customWidth="1"/>
+    <col min="11" max="11" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="7" customFormat="1">

</xml_diff>